<commit_message>
updated error in file
</commit_message>
<xml_diff>
--- a/Robbie Robot Shop Scrum.xlsx
+++ b/Robbie Robot Shop Scrum.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelvu/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelvu/Documents/CSE1325/ROBOT/Robbie_Robot_Shop/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="14560" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="14500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -530,11 +530,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="176077744"/>
-        <c:axId val="176088864"/>
+        <c:axId val="-251494864"/>
+        <c:axId val="-288007008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="176077744"/>
+        <c:axId val="-251494864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -576,7 +576,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="176088864"/>
+        <c:crossAx val="-288007008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -584,7 +584,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="176088864"/>
+        <c:axId val="-288007008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -641,7 +641,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="176077744"/>
+        <c:crossAx val="-251494864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -759,11 +759,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="172427888"/>
-        <c:axId val="110485856"/>
+        <c:axId val="-327391744"/>
+        <c:axId val="-327387712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="172427888"/>
+        <c:axId val="-327391744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -803,7 +803,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="110485856"/>
+        <c:crossAx val="-327387712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -811,7 +811,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110485856"/>
+        <c:axId val="-327387712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -866,7 +866,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="172427888"/>
+        <c:crossAx val="-327391744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1228,7 +1228,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>

</xml_diff>